<commit_message>
aula 07 - atualização
</commit_message>
<xml_diff>
--- a/img/aula07/Exercício-DBC.xlsx
+++ b/img/aula07/Exercício-DBC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\experimentacao-agricola-unesp-fcav\img\aula07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\experimentacao-agricola-unesp-fcav\img\aula07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA695A5C-1942-4BF4-BFC5-1907654ABD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48069A5-3C77-4F6F-9DB0-422DCA8577EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{94995987-2730-4B5A-96B7-995DEF988FAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{94995987-2730-4B5A-96B7-995DEF988FAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>T1</t>
   </si>
@@ -61,6 +61,48 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Exemplo: Efeito da aplicação de Promalin na produção da macieira.</t>
+  </si>
+  <si>
+    <t>TOTAL TR</t>
+  </si>
+  <si>
+    <t>TOTAL BL</t>
+  </si>
+  <si>
+    <t>FV</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>QM</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Fc5%</t>
+  </si>
+  <si>
+    <t>Fc1%</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -70,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,16 +131,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,8 +151,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -169,15 +209,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -208,19 +239,86 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -232,18 +330,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,132 +684,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F19A5C2-228B-4CEB-B963-ACE8DBCE6EF0}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="1">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E3" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B4" s="24">
         <v>142.4</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C4" s="24">
         <v>144.80000000000001</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D4" s="24">
         <v>145.19999999999999</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E4" s="13">
         <v>138.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B5" s="24">
         <v>139.30000000000001</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C5" s="24">
         <v>137.80000000000001</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D5" s="24">
         <v>144.4</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E5" s="13">
         <v>130.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B6" s="24">
         <v>140.69999999999999</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C6" s="24">
         <v>134.1</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D6" s="24">
         <v>136.1</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E6" s="13">
         <v>144.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B7" s="24">
         <v>150.9</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C7" s="24">
         <v>135.80000000000001</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D7" s="24">
         <v>137</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E7" s="13">
         <v>136.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B8" s="13">
         <v>153.5</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C8" s="13">
         <v>165</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D8" s="13">
         <v>151.80000000000001</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E8" s="13">
         <v>150.19999999999999</v>
       </c>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="e">
+        <f>_xlfn.F.INV(0.95,$B12,$B$14)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G12" t="e">
+        <f>_xlfn.F.INV(0.99,$B12,$B$14)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="e">
+        <f>_xlfn.F.INV(0.95,$B13,$B$14)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G13" t="e">
+        <f>_xlfn.F.INV(0.99,$B13,$B$14)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -711,136 +908,223 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E26E36-B12E-470C-A7F9-CB2AA7CB0AB1}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="1">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E3" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B4" s="3">
         <v>142.4</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C4" s="3">
         <v>144.80000000000001</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D4" s="3">
         <v>145.19999999999999</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E4" s="4">
         <v>138.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B5" s="3">
         <v>139.30000000000001</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C5" s="3">
         <v>137.80000000000001</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D5" s="3">
         <v>144.4</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E5" s="4">
         <v>130.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B6" s="3">
         <v>140.69999999999999</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C6" s="3">
         <v>134.1</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D6" s="3">
         <v>136.1</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E6" s="4">
         <v>144.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B7" s="3">
         <v>150.9</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C7" s="3">
         <v>135.80000000000001</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D7" s="3">
         <v>137</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E7" s="4">
         <v>136.4</v>
       </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B8" s="5">
         <v>153.5</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D8" s="5">
         <v>151.80000000000001</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E8" s="6">
         <v>150.19999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="15"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="e">
+        <f>_xlfn.F.INV(0.95,$B12,$B$14)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G12" t="e">
+        <f>_xlfn.F.INV(0.99,$B12,$B$14)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="e">
+        <f>_xlfn.F.INV(0.95,$B13,$B$14)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G13" t="e">
+        <f>_xlfn.F.INV(0.99,$B13,$B$14)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
atualização do exercicio aula 07
</commit_message>
<xml_diff>
--- a/img/aula07/Exercício-DBC.xlsx
+++ b/img/aula07/Exercício-DBC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\experimentacao-agricola-unesp-fcav\img\aula07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48069A5-3C77-4F6F-9DB0-422DCA8577EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA19804-7B13-48FB-8C9E-EF977BD58B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{94995987-2730-4B5A-96B7-995DEF988FAF}"/>
   </bookViews>
@@ -321,6 +321,15 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -330,26 +339,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,7 +687,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A11" sqref="A11:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,21 +701,21 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="19" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -728,173 +728,173 @@
       <c r="E3" s="1">
         <v>4</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="8">
         <v>142.4</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="8">
         <v>144.80000000000001</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="8">
         <v>145.19999999999999</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="8">
         <v>138.9</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="8">
         <v>139.30000000000001</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="8">
         <v>137.80000000000001</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="8">
         <v>144.4</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="8">
         <v>130.6</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="8">
         <v>140.69999999999999</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="8">
         <v>134.1</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="8">
         <v>136.1</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="8">
         <v>144.1</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="8">
         <v>150.9</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="8">
         <v>135.80000000000001</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="8">
         <v>137</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="8">
         <v>136.4</v>
       </c>
-      <c r="F7" s="17"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="8">
         <v>153.5</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="8">
         <v>165</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="8">
         <v>151.80000000000001</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="8">
         <v>150.19999999999999</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="18"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F12" t="e">
-        <f>_xlfn.F.INV(0.95,$B12,$B$14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G12" t="e">
-        <f>_xlfn.F.INV(0.99,$B12,$B$14)</f>
-        <v>#NUM!</v>
+      <c r="F12" s="24" t="str">
+        <f>IFERROR("",_xlfn.F.INV(0.95,$B12,$B$14))</f>
+        <v/>
+      </c>
+      <c r="G12" s="24" t="str">
+        <f>IFERROR("",_xlfn.F.INV(0.99,$B12,$B$14))</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F13" t="e">
-        <f>_xlfn.F.INV(0.95,$B13,$B$14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G13" t="e">
-        <f>_xlfn.F.INV(0.99,$B13,$B$14)</f>
-        <v>#NUM!</v>
+      <c r="F13" s="24" t="str">
+        <f>IFERROR("",_xlfn.F.INV(0.95,$B13,$B$14))</f>
+        <v/>
+      </c>
+      <c r="G13" s="24" t="str">
+        <f>IFERROR("",_xlfn.F.INV(0.99,$B13,$B$14))</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -925,21 +925,21 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="19" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -952,10 +952,10 @@
       <c r="E3" s="2">
         <v>4</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3">
@@ -970,10 +970,10 @@
       <c r="E4" s="4">
         <v>138.9</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3">
@@ -988,10 +988,10 @@
       <c r="E5" s="4">
         <v>130.6</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3">
@@ -1006,10 +1006,10 @@
       <c r="E6" s="4">
         <v>144.1</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="3">
@@ -1024,10 +1024,10 @@
       <c r="E7" s="4">
         <v>136.4</v>
       </c>
-      <c r="F7" s="17"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="5">
@@ -1042,83 +1042,83 @@
       <c r="E8" s="6">
         <v>150.19999999999999</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="18"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F12" t="e">
-        <f>_xlfn.F.INV(0.95,$B12,$B$14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G12" t="e">
-        <f>_xlfn.F.INV(0.99,$B12,$B$14)</f>
-        <v>#NUM!</v>
+      <c r="F12" s="24" t="str">
+        <f>IFERROR("",_xlfn.F.INV(0.95,$B12,$B$14))</f>
+        <v/>
+      </c>
+      <c r="G12" s="24" t="str">
+        <f>IFERROR("",_xlfn.F.INV(0.99,$B12,$B$14))</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F13" t="e">
-        <f>_xlfn.F.INV(0.95,$B13,$B$14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G13" t="e">
-        <f>_xlfn.F.INV(0.99,$B13,$B$14)</f>
-        <v>#NUM!</v>
+      <c r="F13" s="24" t="str">
+        <f>IFERROR("",_xlfn.F.INV(0.95,$B13,$B$14))</f>
+        <v/>
+      </c>
+      <c r="G13" s="24" t="str">
+        <f>IFERROR("",_xlfn.F.INV(0.99,$B13,$B$14))</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
aulas 7 e 8
</commit_message>
<xml_diff>
--- a/img/aula07/Exercício-DBC.xlsx
+++ b/img/aula07/Exercício-DBC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\experimentacao-agricola-unesp-fcav\img\aula07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD70A115-2EAB-41D0-9C79-D9397F59E512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A286D33-9948-4200-BA58-578E1ADEA5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{94995987-2730-4B5A-96B7-995DEF988FAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{94995987-2730-4B5A-96B7-995DEF988FAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>T1</t>
   </si>
@@ -61,13 +61,55 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>FV</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>QM</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Fc5%</t>
+  </si>
+  <si>
+    <t>Fc1%</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>TOTAL B</t>
+  </si>
+  <si>
+    <t>TOTAL T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +127,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -107,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -181,6 +231,71 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -188,47 +303,43 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -565,132 +676,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F19A5C2-228B-4CEB-B963-ACE8DBCE6EF0}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8">
-        <v>142.36000000000001</v>
-      </c>
-      <c r="C3" s="8">
-        <v>144.78</v>
-      </c>
-      <c r="D3" s="8">
-        <v>145.19</v>
-      </c>
-      <c r="E3" s="9">
-        <v>138.88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="5">
+        <v>142.4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>144.80000000000001</v>
+      </c>
+      <c r="D3" s="5">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="E3" s="10">
+        <v>138.9</v>
+      </c>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
-        <v>139.28</v>
-      </c>
-      <c r="C4" s="8">
-        <v>137.77000000000001</v>
-      </c>
-      <c r="D4" s="8">
-        <v>144.44</v>
-      </c>
-      <c r="E4" s="9">
-        <v>130.61000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="5">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="C4" s="5">
+        <v>137.80000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <v>144.4</v>
+      </c>
+      <c r="E4" s="10">
+        <v>130.6</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8">
-        <v>140.72999999999999</v>
-      </c>
-      <c r="C5" s="8">
-        <v>134.06</v>
-      </c>
-      <c r="D5" s="8">
-        <v>136.07</v>
-      </c>
-      <c r="E5" s="9">
-        <v>144.11000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B5" s="5">
+        <v>140.69999999999999</v>
+      </c>
+      <c r="C5" s="5">
+        <v>134.1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>136.1</v>
+      </c>
+      <c r="E5" s="10">
+        <v>144.1</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8">
-        <v>150.88</v>
-      </c>
-      <c r="C6" s="8">
-        <v>135.83000000000001</v>
-      </c>
-      <c r="D6" s="8">
-        <v>136.97</v>
-      </c>
-      <c r="E6" s="9">
-        <v>136.36000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="B6" s="5">
+        <v>150.9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>135.80000000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <v>137</v>
+      </c>
+      <c r="E6" s="10">
+        <v>136.4</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11">
-        <v>153.49</v>
-      </c>
-      <c r="C7" s="11">
-        <v>152.08000000000001</v>
-      </c>
-      <c r="D7" s="11">
-        <v>151.75</v>
-      </c>
-      <c r="E7" s="12">
-        <v>150.22</v>
-      </c>
+      <c r="B7" s="10">
+        <v>153.5</v>
+      </c>
+      <c r="C7" s="10">
+        <v>165</v>
+      </c>
+      <c r="D7" s="10">
+        <v>151.80000000000001</v>
+      </c>
+      <c r="E7" s="10">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -698,10 +895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E26E36-B12E-470C-A7F9-CB2AA7CB0AB1}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,122 +906,207 @@
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8">
-        <v>142.36000000000001</v>
-      </c>
-      <c r="C3" s="8">
-        <v>144.78</v>
-      </c>
-      <c r="D3" s="8">
-        <v>145.19</v>
-      </c>
-      <c r="E3" s="9">
-        <v>138.88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="5">
+        <v>142.4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>144.80000000000001</v>
+      </c>
+      <c r="D3" s="5">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="E3" s="10">
+        <v>138.9</v>
+      </c>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
-        <v>139.28</v>
-      </c>
-      <c r="C4" s="8">
-        <v>137.77000000000001</v>
-      </c>
-      <c r="D4" s="8">
-        <v>144.44</v>
-      </c>
-      <c r="E4" s="9">
-        <v>130.61000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="5">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="C4" s="5">
+        <v>137.80000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <v>144.4</v>
+      </c>
+      <c r="E4" s="10">
+        <v>130.6</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8">
-        <v>140.72999999999999</v>
-      </c>
-      <c r="C5" s="8">
-        <v>134.06</v>
-      </c>
-      <c r="D5" s="8">
-        <v>136.07</v>
-      </c>
-      <c r="E5" s="9">
-        <v>144.11000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B5" s="5">
+        <v>140.69999999999999</v>
+      </c>
+      <c r="C5" s="5">
+        <v>134.1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>136.1</v>
+      </c>
+      <c r="E5" s="10">
+        <v>144.1</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8">
-        <v>150.88</v>
-      </c>
-      <c r="C6" s="8">
-        <v>135.83000000000001</v>
-      </c>
-      <c r="D6" s="8">
-        <v>136.97</v>
-      </c>
-      <c r="E6" s="9">
-        <v>136.36000000000001</v>
-      </c>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="B6" s="5">
+        <v>150.9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>135.80000000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <v>137</v>
+      </c>
+      <c r="E6" s="10">
+        <v>136.4</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11">
-        <v>153.49</v>
-      </c>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="10">
+        <v>153.5</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="11">
-        <v>151.75</v>
-      </c>
-      <c r="E7" s="12">
-        <v>150.22</v>
-      </c>
+      <c r="D7" s="10">
+        <v>151.80000000000001</v>
+      </c>
+      <c r="E7" s="10">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>